<commit_message>
population and inactivity work
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkosf\Documents\nss\projects\smile-on-spiderman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490B1C02-4342-4164-9813-37CB96F875FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A420B1D8-46DC-4455-9186-D61A8F907672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6672" yWindow="2184" windowWidth="14628" windowHeight="9756" xr2:uid="{1456EB46-2F1A-4359-8804-70950F946C77}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1456EB46-2F1A-4359-8804-70950F946C77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,6 +694,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,6 +725,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8352A6-6A43-4B39-A35C-B4C8BC87CC9C}">
   <dimension ref="A1:B183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,7 +2056,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="8" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2074,12 +2081,12 @@
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="8" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>